<commit_message>
updating size; updating dependency versions
</commit_message>
<xml_diff>
--- a/docs/sizes.xlsx
+++ b/docs/sizes.xlsx
@@ -8,17 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timveil/dev/projects/personal/hive-jdbc/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33EFE9A3-8075-7446-9EC1-E8AF3A4E4269}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B501CE-0384-ED45-8B7E-B6F2935F7307}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{9E1AE3AE-99DF-E04B-9E10-857BE9C5B2ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1:$A$4</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$1:$B$4</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -182,6 +178,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-5B3E-6D4F-AD59-7BA2C4BD91E1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -196,6 +197,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-5B3E-6D4F-AD59-7BA2C4BD91E1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -210,6 +216,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-5B3E-6D4F-AD59-7BA2C4BD91E1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -224,6 +235,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-5B3E-6D4F-AD59-7BA2C4BD91E1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -261,7 +277,7 @@
                   <c:v>15.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.6</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1292,7 +1308,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1329,7 +1345,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>12.6</v>
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>